<commit_message>
fix format upload file
</commit_message>
<xml_diff>
--- a/public/src/format_upload.xlsx
+++ b/public/src/format_upload.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevingiovanni/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nakama/Documents/Work/Tokopedia/outside/margamulya/public/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68753759-92D3-A94C-90A8-2B90EDF8FAE2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16440" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,30 +28,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>qty</t>
-  </si>
-  <si>
-    <t>nama_barang</t>
-  </si>
-  <si>
-    <t>harga</t>
-  </si>
-  <si>
-    <t>harga_jual</t>
-  </si>
-  <si>
-    <t>jenis</t>
-  </si>
-  <si>
-    <t>kategori</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>nama</t>
+  </si>
+  <si>
+    <t>tgl_lahir</t>
+  </si>
+  <si>
+    <t>jenis_kelamin</t>
+  </si>
+  <si>
+    <t>alamat</t>
+  </si>
+  <si>
+    <t>sektor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -80,8 +78,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -91,6 +90,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -358,37 +360,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>